<commit_message>
final code for any excel file
</commit_message>
<xml_diff>
--- a/JAN-22/converted.xlsx
+++ b/JAN-22/converted.xlsx
@@ -486,17 +486,17 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Mould Broken</t>
+          <t>Core shift</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Cold Metal</t>
+          <t>Dirt</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>HARD WELD</t>
+          <t>Scab</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
@@ -506,29 +506,31 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>C/Tilt</t>
+          <t>M/br.</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Bed/Core</t>
+          <t>S/POUR</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1-JAN-22</t>
+          <t>1- JAN-22</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
@@ -546,17 +548,19 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2-JAN-22</t>
+          <t>2- JAN-22</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
@@ -574,17 +578,19 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3-JAN-22</t>
+          <t>3- JAN-22</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
@@ -602,17 +608,19 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4-JAN-22</t>
+          <t>4- JAN-22</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
@@ -630,19 +638,25 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5-JAN-22</t>
+          <t>5- JAN-22</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>64</v>
+      </c>
+      <c r="D6" t="n">
+        <v>45</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.03125</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
@@ -651,24 +665,30 @@
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
+      <c r="N6" t="n">
+        <v>1</v>
+      </c>
       <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
+      <c r="P6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>6-JAN-22</t>
+          <t>6- JAN-22</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
@@ -686,17 +706,19 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>7-JAN-22</t>
+          <t>7- JAN-22</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
@@ -714,21 +736,19 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>8-JAN-22</t>
+          <t>8- JAN-22</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>104</v>
-      </c>
-      <c r="D9" t="n">
-        <v>101</v>
-      </c>
-      <c r="E9" t="inlineStr"/>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
@@ -746,12 +766,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>9-JAN-22</t>
+          <t>9- JAN-22</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -776,21 +796,25 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>10-JAN-22</t>
+          <t>10- JAN-22</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>159</v>
+      </c>
+      <c r="D11" t="n">
+        <v>124</v>
+      </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>0.006289308176100629</v>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
@@ -799,19 +823,21 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
+      <c r="N11" t="n">
+        <v>1</v>
+      </c>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>11-JAN-22</t>
+          <t>11- JAN-22</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -836,12 +862,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>12-JAN-22</t>
+          <t>12- JAN-22</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -866,12 +892,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>13-JAN-22</t>
+          <t>13- JAN-22</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -896,12 +922,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>14-JAN-22</t>
+          <t>14- JAN-22</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
@@ -926,12 +952,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>15-JAN-22</t>
+          <t>15- JAN-22</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -956,12 +982,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>16-JAN-22</t>
+          <t>16- JAN-22</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -986,12 +1012,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>17-JAN-22</t>
+          <t>17- JAN-22</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -1016,12 +1042,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>18-JAN-22</t>
+          <t>18- JAN-22</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
@@ -1046,31 +1072,29 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>19-JAN-22</t>
+          <t>19- JAN-22</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.009900990099009901</v>
+        <v>0</v>
       </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
-      <c r="K20" t="n">
-        <v>1</v>
-      </c>
+      <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
@@ -1080,12 +1104,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20-JAN-22</t>
+          <t>20- JAN-22</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
@@ -1110,12 +1134,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>21-JAN-22</t>
+          <t>21- JAN-22</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
@@ -1140,12 +1164,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>22-JAN-22</t>
+          <t>22- JAN-22</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
@@ -1170,12 +1194,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>23-JAN-22</t>
+          <t>23- JAN-22</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
@@ -1200,12 +1224,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>24-JAN-22</t>
+          <t>24- JAN-22</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
@@ -1230,12 +1254,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>25-JAN-22</t>
+          <t>25- JAN-22</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
@@ -1264,12 +1288,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>26-JAN-22</t>
+          <t>26- JAN-22</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
@@ -1294,12 +1318,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>27-JAN-22</t>
+          <t>27- JAN-22</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
@@ -1324,15 +1348,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>28-JAN-22</t>
+          <t>28- JAN-22</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr"/>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>63</v>
+      </c>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="n">
         <v>0</v>
@@ -1354,12 +1380,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>29-JAN-22</t>
+          <t>29- JAN-22</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
@@ -1384,12 +1410,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>30-JAN-22</t>
+          <t>30- JAN-22</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>

</xml_diff>